<commit_message>
v2. Ready for production. Need panic factor
</commit_message>
<xml_diff>
--- a/panic_modal_sum.xlsx
+++ b/panic_modal_sum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF517346-E7AB-4092-88C1-3C53C5CA74B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7326CFD4-75AA-437D-B9A4-81ADD06B85EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:B291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>